<commit_message>
voy agregando autos cambio script simplifico excel
</commit_message>
<xml_diff>
--- a/filter-kits.xlsx
+++ b/filter-kits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihour\Desktop\repos\renova\renova-product-quotator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F92F23-855D-4C4C-9614-D61A89F87619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFAF6F2-8668-4A55-A97C-2AB2BDDE1F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -98,6 +98,36 @@
   </si>
   <si>
     <t>desde 2015</t>
+  </si>
+  <si>
+    <t>Chevrolet Corsa</t>
+  </si>
+  <si>
+    <t>Corsa Classic</t>
+  </si>
+  <si>
+    <t>https://s2.glbimg.com/nFF9NwKwQwBb6LmPpK7bPBzm4ho=/620x465/s.glbimg.com/jo/g1/f/original/2014/06/04/classic_2015.jpg</t>
+  </si>
+  <si>
+    <t>PH4701</t>
+  </si>
+  <si>
+    <t>CA5496</t>
+  </si>
+  <si>
+    <t>G5995</t>
+  </si>
+  <si>
+    <t>HK301</t>
+  </si>
+  <si>
+    <t>Chevrolet</t>
+  </si>
+  <si>
+    <t>Agile/Astra/Celta/Classic/Corsa</t>
+  </si>
+  <si>
+    <t>detail</t>
   </si>
 </sst>
 </file>
@@ -504,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -518,7 +548,7 @@
     <col min="5" max="9" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,8 +582,11 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -588,7 +621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -623,10 +656,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="1"/>
+    <row r="4" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G5" s="1"/>
     </row>
   </sheetData>

</xml_diff>